<commit_message>
few runs & few updates on Click and excel test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestDataNew.xlsx
+++ b/src/test/resources/testdata/TestDataNew.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>firstName</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Dollar</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>Rupee</t>
   </si>
 </sst>
 </file>
@@ -388,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +418,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -417,8 +432,11 @@
       <c r="C2" s="1">
         <v>8767</v>
       </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -428,8 +446,11 @@
       <c r="C3">
         <v>8768</v>
       </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -439,8 +460,11 @@
       <c r="C4">
         <v>8769</v>
       </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -449,6 +473,9 @@
       </c>
       <c r="C5">
         <v>8770</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>